<commit_message>
Dashboard automation framework updates
</commit_message>
<xml_diff>
--- a/Testdata/DSAlgo_Datadriven_Testing_TestNG.xlsx
+++ b/Testdata/DSAlgo_Datadriven_Testing_TestNG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayat\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayat\intellij-learning\DSAlgoProject_TestNG\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6300336D-1FE4-425B-B120-939A0DC82379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F306BFA4-E53B-4996-B559-7EA1816E79CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{859E39E0-2B91-473D-B95C-0EC9B81C152A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>PageTitle</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Get Started</t>
   </si>
   <si>
-    <t>NumpyNinja</t>
-  </si>
-  <si>
     <t>Arrays</t>
   </si>
   <si>
@@ -70,6 +67,27 @@
   </si>
   <si>
     <t>Graph</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TestCaseId</t>
+  </si>
+  <si>
+    <t>TC_Dashboard_001</t>
+  </si>
+  <si>
+    <t>TC_Dashboard_002</t>
+  </si>
+  <si>
+    <t>TC_Dashboard_003</t>
   </si>
 </sst>
 </file>
@@ -136,8 +154,12 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,79 +474,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FD2AFC-7C28-487F-B7B9-F935AAE3FA14}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
-    <col min="2" max="2" width="26.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>